<commit_message>
all the files have been uploaded successfully
</commit_message>
<xml_diff>
--- a/src/main/resources/trello.xlsx
+++ b/src/main/resources/trello.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18072" windowHeight="7716" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14988" windowHeight="7716" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dobData" sheetId="1" r:id="rId1"/>
@@ -702,7 +702,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,7 +781,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>